<commit_message>
code commented on 16th May 2022
</commit_message>
<xml_diff>
--- a/Portal/Content/Uploads/PM_RY.xlsx
+++ b/Portal/Content/Uploads/PM_RY.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$164</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1694,13 +1697,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -9424,6 +9430,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R164"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>